<commit_message>
Little changes in table and adding the header
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Лист1!$A:$H</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -58,10 +61,7 @@
     <t xml:space="preserve">2 метра</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">files/photo.jpg</t>
+    <t xml:space="preserve">files/1.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">б</t>
@@ -76,6 +76,9 @@
     <t xml:space="preserve">1 куст</t>
   </si>
   <si>
+    <t xml:space="preserve">files/2.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">в</t>
   </si>
   <si>
@@ -88,7 +91,43 @@
     <t xml:space="preserve">0.4 милиметра</t>
   </si>
   <si>
-    <t xml:space="preserve">0.1</t>
+    <t xml:space="preserve">files/3.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">г</t>
+  </si>
+  <si>
+    <t xml:space="preserve">табуретка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123 дециметра</t>
+  </si>
+  <si>
+    <t xml:space="preserve">files/4.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">д</t>
+  </si>
+  <si>
+    <t xml:space="preserve">асфальт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 фунт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">files/5.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">е</t>
+  </si>
+  <si>
+    <t xml:space="preserve">диван</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 километра</t>
+  </si>
+  <si>
+    <t xml:space="preserve">files/6.jpg</t>
   </si>
 </sst>
 </file>
@@ -98,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,6 +162,14 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -174,12 +221,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -192,7 +247,28 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -203,12 +279,17 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.42"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -234,7 +315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
@@ -250,43 +331,43 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
@@ -302,11 +383,11 @@
       <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>3</v>
@@ -314,83 +395,84 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>13</v>
+      <c r="F5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>13</v>
+      <c r="F6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>13</v>
+      <c r="F7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="H7" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A:H"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -398,5 +480,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>